<commit_message>
Implemented HOLOVIEWSMAPPING flag for holoviews vs geoviews mapping
Finished and implemented current examination of holoviews-based mapping. Results are mixed. See my notes.
</commit_message>
<xml_diff>
--- a/mbdata_dielcoll_pts_df.xlsx
+++ b/mbdata_dielcoll_pts_df.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,30 +481,40 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>longitude_min</t>
+          <t>londeg</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>longitude_max</t>
+          <t>latdeg</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>latitude_min</t>
+          <t>londeg_min</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>latitude_max</t>
+          <t>londeg_max</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>latdeg_min</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>latdeg_max</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>date_time_min</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>date_time_max</t>
         </is>
@@ -549,21 +559,27 @@
         <v>557</v>
       </c>
       <c r="J2" t="n">
+        <v>-50.16833304781012</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.7630311635190005</v>
+      </c>
+      <c r="L2" t="n">
         <v>-50.1684505586</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>-50.1682337187</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>0.7629053620999999</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>0.7630917756</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="P2" s="2" t="n">
         <v>43558.64930555555</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="Q2" s="2" t="n">
         <v>43559.20277777778</v>
       </c>
     </row>
@@ -606,21 +622,27 @@
         <v>4</v>
       </c>
       <c r="J3" t="n">
+        <v>-50.16836131572499</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.7629928202416667</v>
+      </c>
+      <c r="L3" t="n">
         <v>-50.1683850121</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>-50.1683351118</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>0.7629751414</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>0.7630167995</v>
       </c>
-      <c r="N3" s="2" t="n">
+      <c r="P3" s="2" t="n">
         <v>43558.63888888889</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="Q3" s="2" t="n">
         <v>43558.64097222222</v>
       </c>
     </row>
@@ -663,21 +685,27 @@
         <v>431</v>
       </c>
       <c r="J4" t="n">
+        <v>-50.48780089371607</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-0.02078436265460169</v>
+      </c>
+      <c r="L4" t="n">
         <v>-50.4878946114</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>-50.4877232015</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>-0.0208970066</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>-0.0206745509</v>
       </c>
-      <c r="N4" s="2" t="n">
+      <c r="P4" s="2" t="n">
         <v>43559.90694444445</v>
       </c>
-      <c r="O4" s="2" t="n">
+      <c r="Q4" s="2" t="n">
         <v>43560.23958333334</v>
       </c>
     </row>
@@ -723,18 +751,24 @@
         <v>-51.0042447411</v>
       </c>
       <c r="K5" t="n">
+        <v>-0.0693363603</v>
+      </c>
+      <c r="L5" t="n">
         <v>-51.0042447411</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
+        <v>-51.0042447411</v>
+      </c>
+      <c r="N5" t="n">
         <v>-0.0693363603</v>
       </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>-0.0693363603</v>
       </c>
-      <c r="N5" s="2" t="n">
+      <c r="P5" s="2" t="n">
         <v>42682.50555555556</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="Q5" s="2" t="n">
         <v>42682.50555555556</v>
       </c>
     </row>
@@ -777,21 +811,27 @@
         <v>2</v>
       </c>
       <c r="J6" t="n">
+        <v>-50.58737342715</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-0.1840201579</v>
+      </c>
+      <c r="L6" t="n">
         <v>-50.587796839</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>-50.5869500153</v>
       </c>
-      <c r="L6" t="n">
+      <c r="N6" t="n">
         <v>-0.1844255067</v>
       </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
         <v>-0.1836148091</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="P6" s="2" t="n">
         <v>42681.29513888889</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="Q6" s="2" t="n">
         <v>42681.34791666667</v>
       </c>
     </row>
@@ -834,21 +874,27 @@
         <v>11</v>
       </c>
       <c r="J7" t="n">
+        <v>-50.59285968371363</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-0.1870226813545455</v>
+      </c>
+      <c r="L7" t="n">
         <v>-50.595413642</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>-50.5879072286</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>-0.1901816111</v>
       </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>-0.1839004643</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="P7" s="2" t="n">
         <v>42681.51180555556</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="Q7" s="2" t="n">
         <v>42681.57083333333</v>
       </c>
     </row>
@@ -891,21 +937,27 @@
         <v>2</v>
       </c>
       <c r="J8" t="n">
+        <v>-50.75042369775</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.24299799465</v>
+      </c>
+      <c r="L8" t="n">
         <v>-50.7504318282</v>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
         <v>-50.7504155673</v>
       </c>
-      <c r="L8" t="n">
+      <c r="N8" t="n">
         <v>0.2429420035</v>
       </c>
-      <c r="M8" t="n">
+      <c r="O8" t="n">
         <v>0.2430539858</v>
       </c>
-      <c r="N8" s="2" t="n">
+      <c r="P8" s="2" t="n">
         <v>42678.81041666667</v>
       </c>
-      <c r="O8" s="2" t="n">
+      <c r="Q8" s="2" t="n">
         <v>42678.8125</v>
       </c>
     </row>
@@ -948,21 +1000,27 @@
         <v>72</v>
       </c>
       <c r="J9" t="n">
+        <v>-50.75053674479537</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.2429444325449075</v>
+      </c>
+      <c r="L9" t="n">
         <v>-50.750719998</v>
       </c>
-      <c r="K9" t="n">
+      <c r="M9" t="n">
         <v>-50.75029951985</v>
       </c>
-      <c r="L9" t="n">
+      <c r="N9" t="n">
         <v>0.2428798936</v>
       </c>
-      <c r="M9" t="n">
+      <c r="O9" t="n">
         <v>0.2430988289</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="P9" s="2" t="n">
         <v>42678.82986111111</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="Q9" s="2" t="n">
         <v>42678.95694444444</v>
       </c>
     </row>
@@ -1005,21 +1063,27 @@
         <v>6</v>
       </c>
       <c r="J10" t="n">
+        <v>-50.39322270313889</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-0.1584188942722222</v>
+      </c>
+      <c r="L10" t="n">
         <v>-50.39326597003333</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>-50.393188661</v>
       </c>
-      <c r="L10" t="n">
+      <c r="N10" t="n">
         <v>-0.1584440377</v>
       </c>
-      <c r="M10" t="n">
+      <c r="O10" t="n">
         <v>-0.15840531325</v>
       </c>
-      <c r="N10" s="2" t="n">
+      <c r="P10" s="2" t="n">
         <v>42679.67152777778</v>
       </c>
-      <c r="O10" s="2" t="n">
+      <c r="Q10" s="2" t="n">
         <v>42680.20763888889</v>
       </c>
     </row>
@@ -1065,18 +1129,24 @@
         <v>-50.3932318278</v>
       </c>
       <c r="K11" t="n">
+        <v>-0.1585065667</v>
+      </c>
+      <c r="L11" t="n">
         <v>-50.3932318278</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
+        <v>-50.3932318278</v>
+      </c>
+      <c r="N11" t="n">
         <v>-0.1585065667</v>
       </c>
-      <c r="M11" t="n">
+      <c r="O11" t="n">
         <v>-0.1585065667</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="P11" s="2" t="n">
         <v>42680.20902777778</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="Q11" s="2" t="n">
         <v>42680.20902777778</v>
       </c>
     </row>
@@ -1119,21 +1189,27 @@
         <v>13</v>
       </c>
       <c r="J12" t="n">
+        <v>-50.65473124886154</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-0.1118641640384615</v>
+      </c>
+      <c r="L12" t="n">
         <v>-50.6547934748</v>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>-50.654681325</v>
       </c>
-      <c r="L12" t="n">
+      <c r="N12" t="n">
         <v>-0.1119221281</v>
       </c>
-      <c r="M12" t="n">
+      <c r="O12" t="n">
         <v>-0.1118250657</v>
       </c>
-      <c r="N12" s="2" t="n">
+      <c r="P12" s="2" t="n">
         <v>42680.76458333333</v>
       </c>
-      <c r="O12" s="2" t="n">
+      <c r="Q12" s="2" t="n">
         <v>42680.87708333333</v>
       </c>
     </row>
@@ -1176,21 +1252,27 @@
         <v>591</v>
       </c>
       <c r="J13" t="n">
+        <v>-50.75172738957988</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.2439073902986125</v>
+      </c>
+      <c r="L13" t="n">
         <v>-50.7521916088</v>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>-50.75045278296667</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>0.2405122015333333</v>
       </c>
-      <c r="M13" t="n">
+      <c r="O13" t="n">
         <v>0.2446986828</v>
       </c>
-      <c r="N13" s="2" t="n">
+      <c r="P13" s="2" t="n">
         <v>42851.77222222222</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="Q13" s="2" t="n">
         <v>42852.19444444445</v>
       </c>
     </row>
@@ -1233,21 +1315,27 @@
         <v>10</v>
       </c>
       <c r="J14" t="n">
+        <v>-50.74430074263167</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.2378208171633334</v>
+      </c>
+      <c r="L14" t="n">
         <v>-50.75049586595</v>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>-50.73586623183333</v>
       </c>
-      <c r="L14" t="n">
+      <c r="N14" t="n">
         <v>0.2351875976</v>
       </c>
-      <c r="M14" t="n">
+      <c r="O14" t="n">
         <v>0.2419105265333333</v>
       </c>
-      <c r="N14" s="2" t="n">
+      <c r="P14" s="2" t="n">
         <v>42852.19513888889</v>
       </c>
-      <c r="O14" s="2" t="n">
+      <c r="Q14" s="2" t="n">
         <v>42852.20138888889</v>
       </c>
     </row>
@@ -1290,21 +1378,27 @@
         <v>209</v>
       </c>
       <c r="J15" t="n">
+        <v>-50.58799918718765</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.1631725157531898</v>
+      </c>
+      <c r="L15" t="n">
         <v>-50.66951863466667</v>
       </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
         <v>-50.48480685800001</v>
       </c>
-      <c r="L15" t="n">
+      <c r="N15" t="n">
         <v>-0.02369056925</v>
       </c>
-      <c r="M15" t="n">
+      <c r="O15" t="n">
         <v>0.3778817597666667</v>
       </c>
-      <c r="N15" s="2" t="n">
+      <c r="P15" s="2" t="n">
         <v>42852.62638888889</v>
       </c>
-      <c r="O15" s="2" t="n">
+      <c r="Q15" s="2" t="n">
         <v>42852.77083333334</v>
       </c>
     </row>
@@ -1347,21 +1441,27 @@
         <v>449</v>
       </c>
       <c r="J16" t="n">
+        <v>-50.39329448282211</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-0.1583322410725761</v>
+      </c>
+      <c r="L16" t="n">
         <v>-50.39512448946667</v>
       </c>
-      <c r="K16" t="n">
+      <c r="M16" t="n">
         <v>-50.3931700531</v>
       </c>
-      <c r="L16" t="n">
+      <c r="N16" t="n">
         <v>-0.1592585631</v>
       </c>
-      <c r="M16" t="n">
+      <c r="O16" t="n">
         <v>-0.1582690654</v>
       </c>
-      <c r="N16" s="2" t="n">
+      <c r="P16" s="2" t="n">
         <v>42853.79166666666</v>
       </c>
-      <c r="O16" s="2" t="n">
+      <c r="Q16" s="2" t="n">
         <v>42854.12569444445</v>
       </c>
     </row>
@@ -1404,21 +1504,27 @@
         <v>91</v>
       </c>
       <c r="J17" t="n">
+        <v>-50.47918510132415</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-0.1593090066845996</v>
+      </c>
+      <c r="L17" t="n">
         <v>-50.527546769</v>
       </c>
-      <c r="K17" t="n">
+      <c r="M17" t="n">
         <v>-50.40619016625</v>
       </c>
-      <c r="L17" t="n">
+      <c r="N17" t="n">
         <v>-0.1900570839666667</v>
       </c>
-      <c r="M17" t="n">
+      <c r="O17" t="n">
         <v>-0.1477379724666667</v>
       </c>
-      <c r="N17" s="2" t="n">
+      <c r="P17" s="2" t="n">
         <v>42854.12916666667</v>
       </c>
-      <c r="O17" s="2" t="n">
+      <c r="Q17" s="2" t="n">
         <v>42854.19236111111</v>
       </c>
     </row>
@@ -1461,21 +1567,27 @@
         <v>585</v>
       </c>
       <c r="J18" t="n">
+        <v>-50.56540822839587</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-0.1925415260330484</v>
+      </c>
+      <c r="L18" t="n">
         <v>-50.56554942389999</v>
       </c>
-      <c r="K18" t="n">
+      <c r="M18" t="n">
         <v>-50.56530743835</v>
       </c>
-      <c r="L18" t="n">
+      <c r="N18" t="n">
         <v>-0.1926362514333333</v>
       </c>
-      <c r="M18" t="n">
+      <c r="O18" t="n">
         <v>-0.1924657635</v>
       </c>
-      <c r="N18" s="2" t="n">
+      <c r="P18" s="2" t="n">
         <v>42854.825</v>
       </c>
-      <c r="O18" s="2" t="n">
+      <c r="Q18" s="2" t="n">
         <v>42855.25208333333</v>
       </c>
     </row>
@@ -1518,21 +1630,27 @@
         <v>467</v>
       </c>
       <c r="J19" t="n">
+        <v>-50.84041753380738</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-0.02317948470252626</v>
+      </c>
+      <c r="L19" t="n">
         <v>-50.99723576566667</v>
       </c>
-      <c r="K19" t="n">
+      <c r="M19" t="n">
         <v>-50.82943042739999</v>
       </c>
-      <c r="L19" t="n">
+      <c r="N19" t="n">
         <v>-0.06401002406666667</v>
       </c>
-      <c r="M19" t="n">
+      <c r="O19" t="n">
         <v>-0.0205070805</v>
       </c>
-      <c r="N19" s="2" t="n">
+      <c r="P19" s="2" t="n">
         <v>42855.83055555556</v>
       </c>
-      <c r="O19" s="2" t="n">
+      <c r="Q19" s="2" t="n">
         <v>42856.24722222222</v>
       </c>
     </row>
@@ -1575,21 +1693,27 @@
         <v>5</v>
       </c>
       <c r="J20" t="n">
+        <v>-51.14026537724001</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-0.05239115284000001</v>
+      </c>
+      <c r="L20" t="n">
         <v>-51.1402877234</v>
       </c>
-      <c r="K20" t="n">
+      <c r="M20" t="n">
         <v>-51.1402509268</v>
       </c>
-      <c r="L20" t="n">
+      <c r="N20" t="n">
         <v>-0.0524042454</v>
       </c>
-      <c r="M20" t="n">
+      <c r="O20" t="n">
         <v>-0.0523758307</v>
       </c>
-      <c r="N20" s="2" t="n">
+      <c r="P20" s="2" t="n">
         <v>42681.86388888889</v>
       </c>
-      <c r="O20" s="2" t="n">
+      <c r="Q20" s="2" t="n">
         <v>42681.94166666667</v>
       </c>
     </row>
@@ -1635,18 +1759,24 @@
         <v>-50.59261966035</v>
       </c>
       <c r="K21" t="n">
+        <v>-0.18581162205</v>
+      </c>
+      <c r="L21" t="n">
         <v>-50.59261966035</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
+        <v>-50.59261966035</v>
+      </c>
+      <c r="N21" t="n">
         <v>-0.18581162205</v>
       </c>
-      <c r="M21" t="n">
+      <c r="O21" t="n">
         <v>-0.18581162205</v>
       </c>
-      <c r="N21" s="2" t="n">
+      <c r="P21" s="2" t="n">
         <v>42855.28333333333</v>
       </c>
-      <c r="O21" s="2" t="n">
+      <c r="Q21" s="2" t="n">
         <v>42855.28333333333</v>
       </c>
     </row>
@@ -1689,21 +1819,27 @@
         <v>449</v>
       </c>
       <c r="J22" t="n">
+        <v>-50.58785221231178</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-0.1809539906504762</v>
+      </c>
+      <c r="L22" t="n">
         <v>-50.59400232506667</v>
       </c>
-      <c r="K22" t="n">
+      <c r="M22" t="n">
         <v>-50.5825630948</v>
       </c>
-      <c r="L22" t="n">
+      <c r="N22" t="n">
         <v>-0.18912075555</v>
       </c>
-      <c r="M22" t="n">
+      <c r="O22" t="n">
         <v>-0.1741269137666667</v>
       </c>
-      <c r="N22" s="2" t="n">
+      <c r="P22" s="2" t="n">
         <v>42855.26666666667</v>
       </c>
-      <c r="O22" s="2" t="n">
+      <c r="Q22" s="2" t="n">
         <v>42855.58680555555</v>
       </c>
     </row>
@@ -1746,21 +1882,27 @@
         <v>21</v>
       </c>
       <c r="J23" t="n">
+        <v>-50.5868048057869</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-0.1788861893202381</v>
+      </c>
+      <c r="L23" t="n">
         <v>-50.58818525634999</v>
       </c>
-      <c r="K23" t="n">
+      <c r="M23" t="n">
         <v>-50.585776569775</v>
       </c>
-      <c r="L23" t="n">
+      <c r="N23" t="n">
         <v>-0.17988972365</v>
       </c>
-      <c r="M23" t="n">
+      <c r="O23" t="n">
         <v>-0.177837854725</v>
       </c>
-      <c r="N23" s="2" t="n">
+      <c r="P23" s="2" t="n">
         <v>42855.68611111111</v>
       </c>
-      <c r="O23" s="2" t="n">
+      <c r="Q23" s="2" t="n">
         <v>42855.7</v>
       </c>
     </row>
@@ -1803,21 +1945,27 @@
         <v>15</v>
       </c>
       <c r="J24" t="n">
+        <v>-50.56745721837667</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-0.1916836154695555</v>
+      </c>
+      <c r="L24" t="n">
         <v>-50.5753687676</v>
       </c>
-      <c r="K24" t="n">
+      <c r="M24" t="n">
         <v>-50.56535412555</v>
       </c>
-      <c r="L24" t="n">
+      <c r="N24" t="n">
         <v>-0.19254157785</v>
       </c>
-      <c r="M24" t="n">
+      <c r="O24" t="n">
         <v>-0.1893247012</v>
       </c>
-      <c r="N24" s="2" t="n">
+      <c r="P24" s="2" t="n">
         <v>42855.25416666667</v>
       </c>
-      <c r="O24" s="2" t="n">
+      <c r="Q24" s="2" t="n">
         <v>42855.26388888889</v>
       </c>
     </row>
@@ -1860,21 +2008,27 @@
         <v>5</v>
       </c>
       <c r="J25" t="n">
+        <v>-50.5938314153</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-0.19208541792</v>
+      </c>
+      <c r="L25" t="n">
         <v>-50.5948725902</v>
       </c>
-      <c r="K25" t="n">
+      <c r="M25" t="n">
         <v>-50.5929268152</v>
       </c>
-      <c r="L25" t="n">
+      <c r="N25" t="n">
         <v>-0.1944485027</v>
       </c>
-      <c r="M25" t="n">
+      <c r="O25" t="n">
         <v>-0.1902281307</v>
       </c>
-      <c r="N25" s="2" t="n">
+      <c r="P25" s="2" t="n">
         <v>42681.37847222222</v>
       </c>
-      <c r="O25" s="2" t="n">
+      <c r="Q25" s="2" t="n">
         <v>42681.38819444444</v>
       </c>
     </row>
@@ -1917,21 +2071,27 @@
         <v>3</v>
       </c>
       <c r="J26" t="n">
+        <v>-50.59511485513334</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-0.1950210146333333</v>
+      </c>
+      <c r="L26" t="n">
         <v>-50.5955759995</v>
       </c>
-      <c r="K26" t="n">
+      <c r="M26" t="n">
         <v>-50.5945612025</v>
       </c>
-      <c r="L26" t="n">
+      <c r="N26" t="n">
         <v>-0.1961657032</v>
       </c>
-      <c r="M26" t="n">
+      <c r="O26" t="n">
         <v>-0.1935855858</v>
       </c>
-      <c r="N26" s="2" t="n">
+      <c r="P26" s="2" t="n">
         <v>42681.38611111111</v>
       </c>
-      <c r="O26" s="2" t="n">
+      <c r="Q26" s="2" t="n">
         <v>42681.39166666667</v>
       </c>
     </row>
@@ -1974,21 +2134,27 @@
         <v>3</v>
       </c>
       <c r="J27" t="n">
+        <v>-51.14034463187222</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-0.05237022417222222</v>
+      </c>
+      <c r="L27" t="n">
         <v>-51.1404377595</v>
       </c>
-      <c r="K27" t="n">
+      <c r="M27" t="n">
         <v>-51.14022505466667</v>
       </c>
-      <c r="L27" t="n">
+      <c r="N27" t="n">
         <v>-0.0526345801</v>
       </c>
-      <c r="M27" t="n">
+      <c r="O27" t="n">
         <v>-0.05217863246666667</v>
       </c>
-      <c r="N27" s="2" t="n">
+      <c r="P27" s="2" t="n">
         <v>42851.58125</v>
       </c>
-      <c r="O27" s="2" t="n">
+      <c r="Q27" s="2" t="n">
         <v>42851.58263888889</v>
       </c>
     </row>
@@ -2031,21 +2197,27 @@
         <v>12</v>
       </c>
       <c r="J28" t="n">
+        <v>-50.75183448731528</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.2442109910875</v>
+      </c>
+      <c r="L28" t="n">
         <v>-50.7521745097</v>
       </c>
-      <c r="K28" t="n">
+      <c r="M28" t="n">
         <v>-50.75159071015</v>
       </c>
-      <c r="L28" t="n">
+      <c r="N28" t="n">
         <v>0.2441158891</v>
       </c>
-      <c r="M28" t="n">
+      <c r="O28" t="n">
         <v>0.2443490736</v>
       </c>
-      <c r="N28" s="2" t="n">
+      <c r="P28" s="2" t="n">
         <v>42851.75902777778</v>
       </c>
-      <c r="O28" s="2" t="n">
+      <c r="Q28" s="2" t="n">
         <v>42851.77083333334</v>
       </c>
     </row>
@@ -2088,21 +2260,27 @@
         <v>222</v>
       </c>
       <c r="J29" t="n">
+        <v>-50.3932789492275</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-0.1583377928225226</v>
+      </c>
+      <c r="L29" t="n">
         <v>-50.39335294625</v>
       </c>
-      <c r="K29" t="n">
+      <c r="M29" t="n">
         <v>-50.39316619745</v>
       </c>
-      <c r="L29" t="n">
+      <c r="N29" t="n">
         <v>-0.1583901839</v>
       </c>
-      <c r="M29" t="n">
+      <c r="O29" t="n">
         <v>-0.158278998</v>
       </c>
-      <c r="N29" s="2" t="n">
+      <c r="P29" s="2" t="n">
         <v>42853.62986111111</v>
       </c>
-      <c r="O29" s="2" t="n">
+      <c r="Q29" s="2" t="n">
         <v>42853.78333333333</v>
       </c>
     </row>
@@ -2145,21 +2323,27 @@
         <v>6</v>
       </c>
       <c r="J30" t="n">
+        <v>-50.59517801739444</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-0.1694529736444444</v>
+      </c>
+      <c r="L30" t="n">
         <v>-50.59668350033333</v>
       </c>
-      <c r="K30" t="n">
+      <c r="M30" t="n">
         <v>-50.5935770273</v>
       </c>
-      <c r="L30" t="n">
+      <c r="N30" t="n">
         <v>-0.1757859438666667</v>
       </c>
-      <c r="M30" t="n">
+      <c r="O30" t="n">
         <v>-0.1632633805333333</v>
       </c>
-      <c r="N30" s="2" t="n">
+      <c r="P30" s="2" t="n">
         <v>42855.71388888889</v>
       </c>
-      <c r="O30" s="2" t="n">
+      <c r="Q30" s="2" t="n">
         <v>42855.71736111111</v>
       </c>
     </row>
@@ -2202,21 +2386,27 @@
         <v>52</v>
       </c>
       <c r="J31" t="n">
+        <v>-50.56548728446474</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-0.1925400435868589</v>
+      </c>
+      <c r="L31" t="n">
         <v>-50.56557409466667</v>
       </c>
-      <c r="K31" t="n">
+      <c r="M31" t="n">
         <v>-50.5653936043</v>
       </c>
-      <c r="L31" t="n">
+      <c r="N31" t="n">
         <v>-0.1926088007</v>
       </c>
-      <c r="M31" t="n">
+      <c r="O31" t="n">
         <v>-0.19250817595</v>
       </c>
-      <c r="N31" s="2" t="n">
+      <c r="P31" s="2" t="n">
         <v>42854.78888888889</v>
       </c>
-      <c r="O31" s="2" t="n">
+      <c r="Q31" s="2" t="n">
         <v>42854.82430555556</v>
       </c>
     </row>
@@ -2259,21 +2449,27 @@
         <v>2</v>
       </c>
       <c r="J32" t="n">
+        <v>-51.00440521258334</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-0.07254739756666666</v>
+      </c>
+      <c r="L32" t="n">
         <v>-51.00449527613333</v>
       </c>
-      <c r="K32" t="n">
+      <c r="M32" t="n">
         <v>-51.00431514903334</v>
       </c>
-      <c r="L32" t="n">
+      <c r="N32" t="n">
         <v>-0.072628716</v>
       </c>
-      <c r="M32" t="n">
+      <c r="O32" t="n">
         <v>-0.07246607913333332</v>
       </c>
-      <c r="N32" s="2" t="n">
+      <c r="P32" s="2" t="n">
         <v>42856.25555555556</v>
       </c>
-      <c r="O32" s="2" t="n">
+      <c r="Q32" s="2" t="n">
         <v>42856.25625</v>
       </c>
     </row>
@@ -2316,21 +2512,27 @@
         <v>2</v>
       </c>
       <c r="J33" t="n">
+        <v>-51.00280313755</v>
+      </c>
+      <c r="K33" t="n">
+        <v>-0.068631568</v>
+      </c>
+      <c r="L33" t="n">
         <v>-51.0035934672</v>
       </c>
-      <c r="K33" t="n">
+      <c r="M33" t="n">
         <v>-51.0020128079</v>
       </c>
-      <c r="L33" t="n">
+      <c r="N33" t="n">
         <v>-0.0691408105</v>
       </c>
-      <c r="M33" t="n">
+      <c r="O33" t="n">
         <v>-0.0681223255</v>
       </c>
-      <c r="N33" s="2" t="n">
+      <c r="P33" s="2" t="n">
         <v>42682.46041666667</v>
       </c>
-      <c r="O33" s="2" t="n">
+      <c r="Q33" s="2" t="n">
         <v>42682.47013888889</v>
       </c>
     </row>
@@ -2373,21 +2575,27 @@
         <v>7</v>
       </c>
       <c r="J34" t="n">
+        <v>-51.00498048656429</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-0.06985691240714287</v>
+      </c>
+      <c r="L34" t="n">
         <v>-51.0063599981</v>
       </c>
-      <c r="K34" t="n">
+      <c r="M34" t="n">
         <v>-51.0037101433</v>
       </c>
-      <c r="L34" t="n">
+      <c r="N34" t="n">
         <v>-0.07019961249999999</v>
       </c>
-      <c r="M34" t="n">
+      <c r="O34" t="n">
         <v>-0.0695499312</v>
       </c>
-      <c r="N34" s="2" t="n">
+      <c r="P34" s="2" t="n">
         <v>42682.56180555555</v>
       </c>
-      <c r="O34" s="2" t="n">
+      <c r="Q34" s="2" t="n">
         <v>42682.57013888889</v>
       </c>
     </row>
@@ -2430,21 +2638,27 @@
         <v>202</v>
       </c>
       <c r="J35" t="n">
+        <v>-51.00557062390163</v>
+      </c>
+      <c r="K35" t="n">
+        <v>-0.0763774730340759</v>
+      </c>
+      <c r="L35" t="n">
         <v>-51.0124092177</v>
       </c>
-      <c r="K35" t="n">
+      <c r="M35" t="n">
         <v>-51.0017073713</v>
       </c>
-      <c r="L35" t="n">
+      <c r="N35" t="n">
         <v>-0.09676882070000001</v>
       </c>
-      <c r="M35" t="n">
+      <c r="O35" t="n">
         <v>-0.0664953142</v>
       </c>
-      <c r="N35" s="2" t="n">
+      <c r="P35" s="2" t="n">
         <v>42682.2875</v>
       </c>
-      <c r="O35" s="2" t="n">
+      <c r="Q35" s="2" t="n">
         <v>42682.67569444444</v>
       </c>
     </row>

</xml_diff>